<commit_message>
Integrate custom validation message into built-in's.
</commit_message>
<xml_diff>
--- a/meta/labels/en/ValidationSampleEn.xlsx
+++ b/meta/labels/en/ValidationSampleEn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/labels/en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38251507-C064-D146-8599-85AD1996DD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8E9F82-C950-8C4D-BCDB-37FC660A61E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="900" windowWidth="25820" windowHeight="14980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
   <si>
     <t>画面ラベル定義書</t>
   </si>
@@ -291,6 +291,21 @@
   </si>
   <si>
     <t>validationSample</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>dapanda</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>"dapanda!"</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>駄パンダ</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ダパンダ </t>
+    </rPh>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1214,8 +1229,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1835,10 +1850,18 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B53" s="55"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="52"/>
-      <c r="E53" s="56"/>
+      <c r="B53" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53" s="56" t="s">
+        <v>67</v>
+      </c>
       <c r="F53" s="57"/>
       <c r="G53" s="57"/>
       <c r="H53" s="58"/>

</xml_diff>

<commit_message>
Now available definition of validations with blancoVeeValidate.
</commit_message>
<xml_diff>
--- a/meta/labels/en/ValidationSampleEn.xlsx
+++ b/meta/labels/en/ValidationSampleEn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/labels/en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8E9F82-C950-8C4D-BCDB-37FC660A61E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2D59E6-E74D-A340-968C-3EB1981A1978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="900" windowWidth="25820" windowHeight="14980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
   <si>
     <t>画面ラベル定義書</t>
   </si>
@@ -305,6 +305,21 @@
     <t>駄パンダ</t>
     <rPh sb="0" eb="1">
       <t xml:space="preserve">ダパンダ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>kopanda</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>"kopanda!"</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>子パンダ</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">コ </t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -1230,7 +1245,7 @@
   <dimension ref="A1:AMJ90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1872,10 +1887,18 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B54" s="55"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="52"/>
-      <c r="E54" s="56"/>
+      <c r="B54" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" s="56" t="s">
+        <v>70</v>
+      </c>
       <c r="F54" s="57"/>
       <c r="G54" s="57"/>
       <c r="H54" s="58"/>

</xml_diff>

<commit_message>
Just for recording: PageTransitData is implementing now. ...Stil exist some bugs.
</commit_message>
<xml_diff>
--- a/meta/labels/en/ValidationSampleEn.xlsx
+++ b/meta/labels/en/ValidationSampleEn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/labels/en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9648D56-FFB9-B848-97CF-1B32B70E1031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7254AC98-45BC-4346-A8A7-F112134896CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10600" yWindow="4860" windowWidth="25820" windowHeight="14980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
   <si>
     <t>画面ラベル定義書</t>
   </si>
@@ -338,6 +338,18 @@
     <rPh sb="27" eb="29">
       <t xml:space="preserve">ユウセｎ </t>
     </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>chartnum</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>チャート番号</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>"Select Chart (1 or 2)"</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1261,8 +1273,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1938,10 +1950,18 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B56" s="69"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="71"/>
-      <c r="E56" s="52"/>
+      <c r="B56" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" s="71" t="s">
+        <v>75</v>
+      </c>
+      <c r="E56" s="52" t="s">
+        <v>74</v>
+      </c>
       <c r="F56" s="53"/>
       <c r="G56" s="53"/>
       <c r="H56" s="59"/>

</xml_diff>